<commit_message>
Se agrega produccion por linea de bebidas
</commit_message>
<xml_diff>
--- a/sigset/documentos/prueba 3.xlsx
+++ b/sigset/documentos/prueba 3.xlsx
@@ -327,7 +327,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -356,6 +356,14 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -756,7 +764,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -897,6 +905,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1191,10 +1200,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:R214"/>
+  <dimension ref="A2:R214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <pane ySplit="4875" topLeftCell="A84" activePane="bottomLeft"/>
+      <selection activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="E90" sqref="E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2680,7 +2691,7 @@
         <v>26</v>
       </c>
       <c r="C73" s="56"/>
-      <c r="D73" s="102">
+      <c r="D73" s="80">
         <v>2</v>
       </c>
       <c r="E73" s="46">
@@ -3268,6 +3279,7 @@
         <v>2</v>
       </c>
       <c r="H87" s="33">
+        <f>E87+0</f>
         <v>1</v>
       </c>
       <c r="I87" s="105">
@@ -3288,21 +3300,21 @@
         <v>2</v>
       </c>
       <c r="N87" s="33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O87" s="105">
         <f>$H$32*M87*N87</f>
-        <v>5959388.3799999999</v>
+        <v>11918776.76</v>
       </c>
       <c r="P87" s="80">
         <v>2</v>
       </c>
       <c r="Q87" s="33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R87" s="105">
         <f>$H$32*P87*Q87</f>
-        <v>5959388.3799999999</v>
+        <v>11918776.76</v>
       </c>
     </row>
     <row r="88" spans="2:18">
@@ -3324,6 +3336,7 @@
         <v>2</v>
       </c>
       <c r="H88" s="33">
+        <f t="shared" ref="H88:H91" si="24">E88+0</f>
         <v>1</v>
       </c>
       <c r="I88" s="105">
@@ -3354,11 +3367,11 @@
         <v>2</v>
       </c>
       <c r="Q88" s="33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R88" s="105">
         <f>$H$39*P88*Q88</f>
-        <v>6194627.3949999996</v>
+        <v>12389254.789999999</v>
       </c>
     </row>
     <row r="89" spans="2:18">
@@ -3380,6 +3393,7 @@
         <v>2</v>
       </c>
       <c r="H89" s="33">
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="I89" s="105">
@@ -3390,31 +3404,31 @@
         <v>2</v>
       </c>
       <c r="K89" s="33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L89" s="105">
         <f>$H$46*J89*K89</f>
-        <v>5645736.3600000003</v>
+        <v>11291472.720000001</v>
       </c>
       <c r="M89" s="80">
         <v>2</v>
       </c>
       <c r="N89" s="33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O89" s="105">
         <f>$H$46*M89*N89</f>
-        <v>5645736.3600000003</v>
+        <v>11291472.720000001</v>
       </c>
       <c r="P89" s="80">
         <v>2</v>
       </c>
       <c r="Q89" s="33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R89" s="105">
         <f>$H$46*P89*Q89</f>
-        <v>5645736.3600000003</v>
+        <v>11291472.720000001</v>
       </c>
     </row>
     <row r="90" spans="2:18">
@@ -3426,51 +3440,52 @@
         <v>2</v>
       </c>
       <c r="E90" s="33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F90" s="105">
         <f>$H$54*D90*E90</f>
-        <v>5096845.3250000002</v>
+        <v>10193690.65</v>
       </c>
       <c r="G90" s="80">
         <v>2</v>
       </c>
       <c r="H90" s="33">
-        <v>1</v>
+        <f t="shared" si="24"/>
+        <v>2</v>
       </c>
       <c r="I90" s="105">
         <f>$H$54*G90*H90</f>
-        <v>5096845.3250000002</v>
+        <v>10193690.65</v>
       </c>
       <c r="J90" s="80">
         <v>2</v>
       </c>
       <c r="K90" s="33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L90" s="105">
         <f>$H$54*J90*K90</f>
-        <v>5096845.3250000002</v>
+        <v>10193690.65</v>
       </c>
       <c r="M90" s="80">
         <v>2</v>
       </c>
       <c r="N90" s="33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O90" s="105">
         <f>$H$54*M90*N90</f>
-        <v>5096845.3250000002</v>
+        <v>10193690.65</v>
       </c>
       <c r="P90" s="80">
         <v>2</v>
       </c>
       <c r="Q90" s="33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R90" s="105">
         <f>$H$54*P90*Q90</f>
-        <v>5096845.3250000002</v>
+        <v>10193690.65</v>
       </c>
     </row>
     <row r="91" spans="2:18" ht="15.75" thickBot="1">
@@ -3491,42 +3506,43 @@
       <c r="G91" s="102">
         <v>2</v>
       </c>
-      <c r="H91" s="46">
-        <v>1</v>
+      <c r="H91" s="33">
+        <f>E91+1</f>
+        <v>2</v>
       </c>
       <c r="I91" s="106">
         <f>$H$62*G91*H91</f>
-        <v>5410497.3449999997</v>
+        <v>10820994.689999999</v>
       </c>
       <c r="J91" s="102">
         <v>2</v>
       </c>
-      <c r="K91" s="46">
-        <v>1</v>
+      <c r="K91" s="33">
+        <v>2</v>
       </c>
       <c r="L91" s="106">
         <f>$H$62*J91*K91</f>
-        <v>5410497.3449999997</v>
+        <v>10820994.689999999</v>
       </c>
       <c r="M91" s="102">
         <v>2</v>
       </c>
       <c r="N91" s="46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O91" s="106">
         <f>$H$62*M91*N91</f>
-        <v>5410497.3449999997</v>
+        <v>10820994.689999999</v>
       </c>
       <c r="P91" s="102">
         <v>2</v>
       </c>
       <c r="Q91" s="46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R91" s="106">
         <f>$H$62*P91*Q91</f>
-        <v>5410497.3449999997</v>
+        <v>10820994.689999999</v>
       </c>
     </row>
     <row r="92" spans="2:18" ht="15.75" thickBot="1">
@@ -3538,31 +3554,31 @@
       <c r="E92" s="53"/>
       <c r="F92" s="54">
         <f>MIN(F87:F91)</f>
-        <v>5096845.3250000002</v>
+        <v>5410497.3449999997</v>
       </c>
       <c r="G92" s="54"/>
       <c r="H92" s="54"/>
       <c r="I92" s="54">
         <f>MIN(I87:I91)</f>
-        <v>5096845.3250000002</v>
+        <v>5645736.3600000003</v>
       </c>
       <c r="J92" s="54"/>
       <c r="K92" s="54"/>
       <c r="L92" s="54">
         <f>MIN(L87:L91)</f>
-        <v>5096845.3250000002</v>
+        <v>5959388.3799999999</v>
       </c>
       <c r="M92" s="54"/>
       <c r="N92" s="54"/>
       <c r="O92" s="54">
         <f>MIN(O87:O91)</f>
-        <v>5096845.3250000002</v>
+        <v>6194627.3949999996</v>
       </c>
       <c r="P92" s="54"/>
       <c r="Q92" s="54"/>
       <c r="R92" s="55">
         <f>MIN(R87:R91)</f>
-        <v>5096845.3250000002</v>
+        <v>10193690.65</v>
       </c>
     </row>
     <row r="93" spans="2:18" ht="15.75" thickBot="1"/>
@@ -3704,7 +3720,8 @@
         <v>6390187.54</v>
       </c>
     </row>
-    <row r="97" spans="2:18">
+    <row r="97" spans="1:18">
+      <c r="A97" s="108"/>
       <c r="B97" s="61" t="s">
         <v>23</v>
       </c>
@@ -3760,7 +3777,7 @@
         <v>6642431.7850000001</v>
       </c>
     </row>
-    <row r="98" spans="2:18">
+    <row r="98" spans="1:18">
       <c r="B98" s="61" t="s">
         <v>24</v>
       </c>
@@ -3816,7 +3833,7 @@
         <v>6053861.8799999999</v>
       </c>
     </row>
-    <row r="99" spans="2:18">
+    <row r="99" spans="1:18">
       <c r="B99" s="61" t="s">
         <v>25</v>
       </c>
@@ -3872,7 +3889,7 @@
         <v>5465291.9749999996</v>
       </c>
     </row>
-    <row r="100" spans="2:18" ht="15.75" thickBot="1">
+    <row r="100" spans="1:18" ht="15.75" thickBot="1">
       <c r="B100" s="61" t="s">
         <v>26</v>
       </c>
@@ -3928,7 +3945,7 @@
         <v>5801617.6349999998</v>
       </c>
     </row>
-    <row r="101" spans="2:18" ht="15.75" thickBot="1">
+    <row r="101" spans="1:18" ht="15.75" thickBot="1">
       <c r="B101" s="103" t="s">
         <v>89</v>
       </c>
@@ -3964,7 +3981,7 @@
         <v>5465291.9749999996</v>
       </c>
     </row>
-    <row r="104" spans="2:18">
+    <row r="104" spans="1:18">
       <c r="B104" s="97" t="s">
         <v>38</v>
       </c>
@@ -3973,40 +3990,40 @@
       <c r="E104" s="97"/>
       <c r="F104" s="97"/>
     </row>
-    <row r="105" spans="2:18">
+    <row r="105" spans="1:18">
       <c r="B105" s="97"/>
       <c r="C105" s="97"/>
       <c r="D105" s="97"/>
       <c r="E105" s="97"/>
       <c r="F105" s="97"/>
     </row>
-    <row r="106" spans="2:18">
+    <row r="106" spans="1:18">
       <c r="B106" s="97"/>
       <c r="C106" s="97"/>
       <c r="D106" s="97"/>
       <c r="E106" s="97"/>
       <c r="F106" s="97"/>
     </row>
-    <row r="107" spans="2:18">
+    <row r="107" spans="1:18">
       <c r="B107" s="97"/>
       <c r="C107" s="97"/>
       <c r="D107" s="97"/>
       <c r="E107" s="97"/>
       <c r="F107" s="97"/>
     </row>
-    <row r="108" spans="2:18">
+    <row r="108" spans="1:18">
       <c r="B108" s="47"/>
       <c r="C108" s="47"/>
       <c r="D108" s="47"/>
       <c r="E108" s="47"/>
       <c r="F108" s="47"/>
     </row>
-    <row r="109" spans="2:18" ht="15.75" thickBot="1">
+    <row r="109" spans="1:18" ht="15.75" thickBot="1">
       <c r="B109" s="28" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="110" spans="2:18">
+    <row r="110" spans="1:18">
       <c r="B110" s="29" t="s">
         <v>27</v>
       </c>
@@ -4027,56 +4044,56 @@
         <v>13</v>
       </c>
     </row>
-    <row r="111" spans="2:18">
+    <row r="111" spans="1:18">
       <c r="B111" s="39" t="s">
         <v>5</v>
       </c>
       <c r="C111" s="37"/>
       <c r="D111" s="5">
-        <f>MIN(F69,F79,F85,F91,F99)</f>
-        <v>5410497.3449999997</v>
+        <f>F$74</f>
+        <v>5219660.875</v>
       </c>
       <c r="E111" s="5">
-        <f>MIN(I69,I79,I85,I91,I99)</f>
-        <v>5410497.3449999997</v>
+        <f>$I$74</f>
+        <v>5219660.875</v>
       </c>
       <c r="F111" s="5">
-        <f>MIN(L69,L79,L85,L91,L99)</f>
-        <v>5410497.3449999997</v>
+        <f>$L$74</f>
+        <v>5219660.875</v>
       </c>
       <c r="G111" s="5">
-        <f>MIN(O69,O79,O85,O91,O99)</f>
-        <v>5410497.3449999997</v>
+        <f>$O$74</f>
+        <v>5219660.875</v>
       </c>
       <c r="H111" s="5">
-        <f>MIN(R69,R79,R85,R91,R99)</f>
-        <v>5410497.3449999997</v>
-      </c>
-    </row>
-    <row r="112" spans="2:18">
+        <f>$R$74</f>
+        <v>5219660.875</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18">
       <c r="B112" s="39" t="s">
         <v>6</v>
       </c>
       <c r="C112" s="37"/>
       <c r="D112" s="5">
-        <f>MIN(F70,F80,F86,F92,F100)</f>
-        <v>5096845.3250000002</v>
+        <f>F83</f>
+        <v>5342476.4249999998</v>
       </c>
       <c r="E112" s="5">
-        <f>MIN(I70,I80,I86,I92,I100)</f>
-        <v>5096845.3250000002</v>
+        <f>$I$83</f>
+        <v>5342476.4249999998</v>
       </c>
       <c r="F112" s="5">
-        <f>MIN(L70,L80,L86,L92,L100)</f>
-        <v>5096845.3250000002</v>
+        <f>$L$83</f>
+        <v>5342476.4249999998</v>
       </c>
       <c r="G112" s="5">
-        <f>MIN(O70,O80,O86,O92,O100)</f>
-        <v>5096845.3250000002</v>
+        <f>$O$83</f>
+        <v>5342476.4249999998</v>
       </c>
       <c r="H112" s="5">
-        <f>MIN(R70,R80,R86,R92,R100)</f>
-        <v>5096845.3250000002</v>
+        <f>$R$83</f>
+        <v>5342476.4249999998</v>
       </c>
     </row>
     <row r="113" spans="2:8">
@@ -4085,24 +4102,24 @@
       </c>
       <c r="C113" s="37"/>
       <c r="D113" s="5">
-        <f>MIN(F71,F81,F87,F93,F101)</f>
-        <v>5342476.4249999998</v>
+        <f>F92</f>
+        <v>5410497.3449999997</v>
       </c>
       <c r="E113" s="5">
-        <f>MIN(I71,I81,I87,I93,I101)</f>
-        <v>5342476.4249999998</v>
+        <f>$I$92</f>
+        <v>5645736.3600000003</v>
       </c>
       <c r="F113" s="5">
-        <f>MIN(L71,L81,L87,L93,L101)</f>
-        <v>5342476.4249999998</v>
+        <f>$L$92</f>
+        <v>5959388.3799999999</v>
       </c>
       <c r="G113" s="5">
-        <f>MIN(O71,O81,O87,O93,O101)</f>
-        <v>5342476.4249999998</v>
+        <f>$O$92</f>
+        <v>6194627.3949999996</v>
       </c>
       <c r="H113" s="5">
-        <f>MIN(R71,R81,R87,R93,R101)</f>
-        <v>5342476.4249999998</v>
+        <f>$R$92</f>
+        <v>10193690.65</v>
       </c>
     </row>
     <row r="114" spans="2:8" ht="15.75" thickBot="1">
@@ -4111,24 +4128,24 @@
       </c>
       <c r="C114" s="37"/>
       <c r="D114" s="35">
-        <f>MIN(F72,F82,F88,F95,F102)</f>
-        <v>5219660.875</v>
-      </c>
-      <c r="E114" s="35">
-        <f>MIN(I72,I82,I88,I95,I102)</f>
-        <v>5219660.875</v>
-      </c>
-      <c r="F114" s="35">
-        <f>MIN(L72,L82,L88,L95,L102)</f>
-        <v>5219660.875</v>
-      </c>
-      <c r="G114" s="35">
-        <f>MIN(O72,O82,O88,O95,O102)</f>
-        <v>5219660.875</v>
-      </c>
-      <c r="H114" s="35">
-        <f>MIN(R72,R82,R88,R95,R102)</f>
-        <v>5219660.875</v>
+        <f>F101</f>
+        <v>5465291.9749999996</v>
+      </c>
+      <c r="E114" s="5">
+        <f>$I$101</f>
+        <v>5465291.9749999996</v>
+      </c>
+      <c r="F114" s="5">
+        <f>$L$101</f>
+        <v>5465291.9749999996</v>
+      </c>
+      <c r="G114" s="5">
+        <f>$O$101</f>
+        <v>5465291.9749999996</v>
+      </c>
+      <c r="H114" s="5">
+        <f>$R$101</f>
+        <v>5465291.9749999996</v>
       </c>
     </row>
     <row r="115" spans="2:8" ht="15.75" thickBot="1">
@@ -4138,23 +4155,23 @@
       <c r="C115" s="49"/>
       <c r="D115" s="50">
         <f>SUM(D111:D114)</f>
-        <v>21069479.969999999</v>
+        <v>21437926.619999997</v>
       </c>
       <c r="E115" s="50">
         <f>SUM(E111:E114)</f>
-        <v>21069479.969999999</v>
+        <v>21673165.634999998</v>
       </c>
       <c r="F115" s="50">
         <f>SUM(F111:F114)</f>
-        <v>21069479.969999999</v>
+        <v>21986817.655000001</v>
       </c>
       <c r="G115" s="50">
         <f>SUM(G111:G114)</f>
-        <v>21069479.969999999</v>
+        <v>22222056.670000002</v>
       </c>
       <c r="H115" s="51">
         <f>SUM(H111:H114)</f>
-        <v>21069479.969999999</v>
+        <v>26221119.925000004</v>
       </c>
     </row>
     <row r="118" spans="2:8">
@@ -4213,23 +4230,23 @@
       <c r="C125" s="37"/>
       <c r="D125" s="5">
         <f>(D111*$F4)*($E$123/100)</f>
-        <v>1149730685.8125</v>
+        <v>1109177935.9375</v>
       </c>
       <c r="E125" s="5">
         <f>(E111*$F4)*($E$123/100)</f>
-        <v>1149730685.8125</v>
+        <v>1109177935.9375</v>
       </c>
       <c r="F125" s="5">
         <f>(F111*$F4)*($E$123/100)</f>
-        <v>1149730685.8125</v>
+        <v>1109177935.9375</v>
       </c>
       <c r="G125" s="5">
         <f>(G111*$F4)*($E$123/100)</f>
-        <v>1149730685.8125</v>
+        <v>1109177935.9375</v>
       </c>
       <c r="H125" s="5">
         <f>(H111*$F4)*($E$123/100)</f>
-        <v>1149730685.8125</v>
+        <v>1109177935.9375</v>
       </c>
     </row>
     <row r="126" spans="2:8">
@@ -4239,23 +4256,23 @@
       <c r="C126" s="37"/>
       <c r="D126" s="5">
         <f>(D112*F5)*(E123/100)</f>
-        <v>1083079631.5625</v>
+        <v>1135276240.3125</v>
       </c>
       <c r="E126" s="5">
         <f>(E112*$F5)*($E$123/100)</f>
-        <v>1083079631.5625</v>
+        <v>1135276240.3125</v>
       </c>
       <c r="F126" s="5">
         <f>(F112*$F5)*($E$123/100)</f>
-        <v>1083079631.5625</v>
+        <v>1135276240.3125</v>
       </c>
       <c r="G126" s="5">
         <f>(G112*$F5)*($E$123/100)</f>
-        <v>1083079631.5625</v>
+        <v>1135276240.3125</v>
       </c>
       <c r="H126" s="5">
         <f>(H112*$F5)*($E$123/100)</f>
-        <v>1083079631.5625</v>
+        <v>1135276240.3125</v>
       </c>
     </row>
     <row r="127" spans="2:8">
@@ -4265,23 +4282,23 @@
       <c r="C127" s="37"/>
       <c r="D127" s="5">
         <f>(D113*F6)*(E123/100)</f>
-        <v>1402400061.5625</v>
+        <v>1420255553.0625</v>
       </c>
       <c r="E127" s="5">
         <f>(E113*$F6)*($E$123/100)</f>
-        <v>1402400061.5625</v>
+        <v>1482005794.5</v>
       </c>
       <c r="F127" s="5">
         <f>(F113*$F6)*($E$123/100)</f>
-        <v>1402400061.5625</v>
+        <v>1564339449.75</v>
       </c>
       <c r="G127" s="5">
         <f>(G113*$F6)*($E$123/100)</f>
-        <v>1402400061.5625</v>
+        <v>1626089691.1875</v>
       </c>
       <c r="H127" s="5">
         <f>(H113*$F6)*($E$123/100)</f>
-        <v>1402400061.5625</v>
+        <v>2675843795.625</v>
       </c>
     </row>
     <row r="128" spans="2:8" ht="15.75" thickBot="1">
@@ -4291,23 +4308,23 @@
       <c r="C128" s="37"/>
       <c r="D128" s="35">
         <f>(D114*F7)*(E123/100)</f>
-        <v>1370160979.6875</v>
+        <v>1434639143.4375</v>
       </c>
       <c r="E128" s="5">
         <f>(E114*$F7)*($E$123/100)</f>
-        <v>1370160979.6875</v>
+        <v>1434639143.4375</v>
       </c>
       <c r="F128" s="5">
         <f>(F114*$F7)*($E$123/100)</f>
-        <v>1370160979.6875</v>
+        <v>1434639143.4375</v>
       </c>
       <c r="G128" s="5">
         <f>(G114*$F7)*($E$123/100)</f>
-        <v>1370160979.6875</v>
+        <v>1434639143.4375</v>
       </c>
       <c r="H128" s="5">
         <f>(H114*$F7)*($E$123/100)</f>
-        <v>1370160979.6875</v>
+        <v>1434639143.4375</v>
       </c>
     </row>
     <row r="129" spans="2:8" ht="15.75" thickBot="1">
@@ -4317,23 +4334,23 @@
       <c r="C129" s="53"/>
       <c r="D129" s="54">
         <f>SUM(D125:D128)</f>
-        <v>5005371358.625</v>
+        <v>5099348872.75</v>
       </c>
       <c r="E129" s="54">
         <f>SUM(E125:E128)</f>
-        <v>5005371358.625</v>
+        <v>5161099114.1875</v>
       </c>
       <c r="F129" s="54">
         <f>SUM(F125:F128)</f>
-        <v>5005371358.625</v>
+        <v>5243432769.4375</v>
       </c>
       <c r="G129" s="54">
         <f>SUM(G125:G128)</f>
-        <v>5005371358.625</v>
+        <v>5305183010.875</v>
       </c>
       <c r="H129" s="55">
         <f>SUM(H125:H128)</f>
-        <v>5005371358.625</v>
+        <v>6354937115.3125</v>
       </c>
     </row>
     <row r="132" spans="2:8" ht="15.75" thickBot="1">
@@ -4397,23 +4414,23 @@
       </c>
       <c r="C135" s="37"/>
       <c r="D135" s="5">
-        <f t="shared" ref="D135:H137" si="24">(C21*($E$132/100))</f>
+        <f t="shared" ref="D135:H137" si="25">(C21*($E$132/100))</f>
         <v>367200000</v>
       </c>
       <c r="E135" s="5">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>376379999.99999994</v>
       </c>
       <c r="F135" s="5">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>385789499.99999988</v>
       </c>
       <c r="G135" s="5">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>395434237.49999988</v>
       </c>
       <c r="H135" s="5">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>405320093.43749982</v>
       </c>
     </row>
@@ -4423,23 +4440,23 @@
       </c>
       <c r="C136" s="37"/>
       <c r="D136" s="5">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>680400000</v>
       </c>
       <c r="E136" s="5">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>711018000</v>
       </c>
       <c r="F136" s="5">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>743013810</v>
       </c>
       <c r="G136" s="5">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>776449431.44999981</v>
       </c>
       <c r="H136" s="5">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>811389655.86524987</v>
       </c>
     </row>
@@ -4449,23 +4466,23 @@
       </c>
       <c r="C137" s="37"/>
       <c r="D137" s="5">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>423360000</v>
       </c>
       <c r="E137" s="5">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>448761600</v>
       </c>
       <c r="F137" s="5">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>475687296</v>
       </c>
       <c r="G137" s="5">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>504228533.76000005</v>
       </c>
       <c r="H137" s="5">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>534482245.78560013</v>
       </c>
     </row>
@@ -4538,15 +4555,15 @@
         <v>118766249.99999997</v>
       </c>
       <c r="F143" s="5">
-        <f t="shared" ref="F143:H143" si="25">(E20*($E$141/100))</f>
+        <f t="shared" ref="F143:H143" si="26">(E20*($E$141/100))</f>
         <v>122923068.74999996</v>
       </c>
       <c r="G143" s="5">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>127225376.15624996</v>
       </c>
       <c r="H143" s="5">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>131678264.32171868</v>
       </c>
     </row>
@@ -4556,23 +4573,23 @@
       </c>
       <c r="C144" s="37"/>
       <c r="D144" s="5">
-        <f t="shared" ref="D144:H146" si="26">(C21*($E$141/100))</f>
+        <f t="shared" ref="D144:H146" si="27">(C21*($E$141/100))</f>
         <v>137700000</v>
       </c>
       <c r="E144" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>141142499.99999997</v>
       </c>
       <c r="F144" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>144671062.49999994</v>
       </c>
       <c r="G144" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>148287839.06249994</v>
       </c>
       <c r="H144" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>151995035.03906244</v>
       </c>
     </row>
@@ -4582,23 +4599,23 @@
       </c>
       <c r="C145" s="37"/>
       <c r="D145" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>255150000</v>
       </c>
       <c r="E145" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>266631750</v>
       </c>
       <c r="F145" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>278630178.75</v>
       </c>
       <c r="G145" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>291168536.79374993</v>
       </c>
       <c r="H145" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>304271120.94946867</v>
       </c>
     </row>
@@ -4608,23 +4625,23 @@
       </c>
       <c r="C146" s="37"/>
       <c r="D146" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>158760000</v>
       </c>
       <c r="E146" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>168285600</v>
       </c>
       <c r="F146" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>178382736</v>
       </c>
       <c r="G146" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>189085700.16000003</v>
       </c>
       <c r="H146" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>200430842.16960004</v>
       </c>
     </row>
@@ -4638,19 +4655,19 @@
         <v>666360000</v>
       </c>
       <c r="E147" s="54">
-        <f t="shared" ref="E147:H147" si="27">SUM(E143:E146)</f>
+        <f t="shared" ref="E147:H147" si="28">SUM(E143:E146)</f>
         <v>694826100</v>
       </c>
       <c r="F147" s="54">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>724607045.99999988</v>
       </c>
       <c r="G147" s="54">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>755767452.1724999</v>
       </c>
       <c r="H147" s="55">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>788375262.47984982</v>
       </c>
     </row>
@@ -4722,18 +4739,18 @@
         <v>250000000</v>
       </c>
       <c r="F153" s="5">
-        <f t="shared" ref="F153:F157" si="28">(E153*D153)</f>
+        <f t="shared" ref="F153:F157" si="29">(E153*D153)</f>
         <v>250000000</v>
       </c>
       <c r="G153" s="5">
         <v>15</v>
       </c>
       <c r="H153" s="5">
-        <f t="shared" ref="H153:H157" si="29">(F153*($H$150/100))</f>
+        <f t="shared" ref="H153:H157" si="30">(F153*($H$150/100))</f>
         <v>37500000</v>
       </c>
       <c r="I153" s="5">
-        <f t="shared" ref="I153:I157" si="30">(F153-H153)/G153</f>
+        <f t="shared" ref="I153:I157" si="31">(F153-H153)/G153</f>
         <v>14166666.666666666</v>
       </c>
     </row>
@@ -4749,18 +4766,18 @@
         <v>130000000</v>
       </c>
       <c r="F154" s="5">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>130000000</v>
       </c>
       <c r="G154" s="5">
         <v>15</v>
       </c>
       <c r="H154" s="5">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>19500000</v>
       </c>
       <c r="I154" s="5">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>7366666.666666667</v>
       </c>
     </row>
@@ -4776,18 +4793,18 @@
         <v>180000000</v>
       </c>
       <c r="F155" s="5">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>360000000</v>
       </c>
       <c r="G155" s="5">
         <v>15</v>
       </c>
       <c r="H155" s="5">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>54000000</v>
       </c>
       <c r="I155" s="5">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>20400000</v>
       </c>
     </row>
@@ -4803,18 +4820,18 @@
         <v>90000000</v>
       </c>
       <c r="F156" s="5">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>90000000</v>
       </c>
       <c r="G156" s="5">
         <v>15</v>
       </c>
       <c r="H156" s="5">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>13500000</v>
       </c>
       <c r="I156" s="5">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>5100000</v>
       </c>
     </row>
@@ -4830,18 +4847,18 @@
         <v>350000000</v>
       </c>
       <c r="F157" s="35">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>350000000</v>
       </c>
       <c r="G157" s="35">
         <v>50</v>
       </c>
       <c r="H157" s="35">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>52500000</v>
       </c>
       <c r="I157" s="5">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>5950000</v>
       </c>
     </row>
@@ -4923,14 +4940,14 @@
         <v>10</v>
       </c>
       <c r="C164" s="5">
-        <f t="shared" ref="C164:C167" si="31">SUM($I$152:$I$157)</f>
+        <f t="shared" ref="C164:C167" si="32">SUM($I$152:$I$157)</f>
         <v>61483333.333333328</v>
       </c>
       <c r="E164" s="59" t="s">
         <v>65</v>
       </c>
       <c r="F164" s="75">
-        <f t="shared" ref="F164:F168" si="32">G164*I153</f>
+        <f t="shared" ref="F164:F168" si="33">G164*I153</f>
         <v>141666666.66666666</v>
       </c>
       <c r="G164" s="24">
@@ -4942,14 +4959,14 @@
         <v>11</v>
       </c>
       <c r="C165" s="5">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>61483333.333333328</v>
       </c>
       <c r="E165" s="59" t="s">
         <v>66</v>
       </c>
       <c r="F165" s="75">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>73666666.666666672</v>
       </c>
       <c r="G165" s="24">
@@ -4961,14 +4978,14 @@
         <v>12</v>
       </c>
       <c r="C166" s="5">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>61483333.333333328</v>
       </c>
       <c r="E166" s="59" t="s">
         <v>67</v>
       </c>
       <c r="F166" s="75">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>204000000</v>
       </c>
       <c r="G166" s="24">
@@ -4980,14 +4997,14 @@
         <v>13</v>
       </c>
       <c r="C167" s="5">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>61483333.333333328</v>
       </c>
       <c r="E167" s="59" t="s">
         <v>68</v>
       </c>
       <c r="F167" s="75">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>51000000</v>
       </c>
       <c r="G167" s="24">
@@ -5001,7 +5018,7 @@
         <v>49</v>
       </c>
       <c r="F168" s="76">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>267750000</v>
       </c>
       <c r="G168" s="27">
@@ -5150,23 +5167,23 @@
         <v>1150000000</v>
       </c>
       <c r="E178" s="72">
-        <f t="shared" ref="E178:I178" si="33">SUM(E172:E177)</f>
+        <f t="shared" ref="E178:I178" si="34">SUM(E172:E177)</f>
         <v>180000000</v>
       </c>
       <c r="F178" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>90000000</v>
       </c>
       <c r="G178" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>130000000</v>
       </c>
       <c r="H178" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>400000000</v>
       </c>
       <c r="I178" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
     </row>
@@ -5444,19 +5461,19 @@
       </c>
       <c r="E198" s="5">
         <f>(E$115*D198)/D$115</f>
-        <v>36250</v>
+        <v>36647.772342675831</v>
       </c>
       <c r="F198" s="5">
-        <f t="shared" ref="F198" si="34">(F$115*E198)/E$115</f>
-        <v>36250</v>
+        <f t="shared" ref="F198" si="35">(F$115*E198)/E$115</f>
+        <v>37178.135466243613</v>
       </c>
       <c r="G198" s="5">
-        <f t="shared" ref="G198:H198" si="35">(G$115*F198)/F$115</f>
-        <v>36250</v>
+        <f t="shared" ref="G198:H198" si="36">(G$115*F198)/F$115</f>
+        <v>37575.907808919445</v>
       </c>
       <c r="H198" s="5">
-        <f t="shared" si="35"/>
-        <v>36250</v>
+        <f t="shared" si="36"/>
+        <v>44338.037634408611</v>
       </c>
     </row>
     <row r="199" spans="2:9">
@@ -5465,24 +5482,24 @@
       </c>
       <c r="C199" s="56"/>
       <c r="D199" s="88">
-        <f t="shared" ref="D199:D202" si="36">I185*($D$196/100)</f>
+        <f t="shared" ref="D199:D202" si="37">I185*($D$196/100)</f>
         <v>43750</v>
       </c>
       <c r="E199" s="5">
-        <f t="shared" ref="E199:F203" si="37">(E$115*D199)/D$115</f>
-        <v>43750</v>
+        <f t="shared" ref="E199:F203" si="38">(E$115*D199)/D$115</f>
+        <v>44230.070068746696</v>
       </c>
       <c r="F199" s="5">
-        <f t="shared" si="37"/>
-        <v>43750</v>
+        <f t="shared" si="38"/>
+        <v>44870.163493742293</v>
       </c>
       <c r="G199" s="5">
-        <f t="shared" ref="G199:H199" si="38">(G$115*F199)/F$115</f>
-        <v>43750</v>
+        <f t="shared" ref="G199:H199" si="39">(G$115*F199)/F$115</f>
+        <v>45350.233562488989</v>
       </c>
       <c r="H199" s="5">
-        <f t="shared" si="38"/>
-        <v>43750</v>
+        <f t="shared" si="39"/>
+        <v>53511.424731182808</v>
       </c>
     </row>
     <row r="200" spans="2:9">
@@ -5491,24 +5508,24 @@
       </c>
       <c r="C200" s="56"/>
       <c r="D200" s="88">
-        <f t="shared" si="36"/>
-        <v>33750</v>
-      </c>
-      <c r="E200" s="5">
         <f t="shared" si="37"/>
         <v>33750</v>
       </c>
+      <c r="E200" s="5">
+        <f t="shared" si="38"/>
+        <v>34120.339767318881</v>
+      </c>
       <c r="F200" s="5">
-        <f t="shared" si="37"/>
-        <v>33750</v>
+        <f t="shared" si="38"/>
+        <v>34614.126123744056</v>
       </c>
       <c r="G200" s="5">
-        <f t="shared" ref="G200:H200" si="39">(G$115*F200)/F$115</f>
-        <v>33750</v>
+        <f t="shared" ref="G200:H200" si="40">(G$115*F200)/F$115</f>
+        <v>34984.465891062937</v>
       </c>
       <c r="H200" s="5">
-        <f t="shared" si="39"/>
-        <v>33750</v>
+        <f t="shared" si="40"/>
+        <v>41280.241935483886</v>
       </c>
     </row>
     <row r="201" spans="2:9">
@@ -5517,24 +5534,24 @@
       </c>
       <c r="C201" s="56"/>
       <c r="D201" s="88">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>32500</v>
       </c>
       <c r="E201" s="5">
-        <f t="shared" si="37"/>
-        <v>32500.000000000004</v>
+        <f t="shared" si="38"/>
+        <v>32856.623479640402</v>
       </c>
       <c r="F201" s="5">
-        <f t="shared" si="37"/>
-        <v>32500.000000000004</v>
+        <f t="shared" si="38"/>
+        <v>33332.121452494277</v>
       </c>
       <c r="G201" s="5">
-        <f t="shared" ref="G201:H201" si="40">(G$115*F201)/F$115</f>
-        <v>32500.000000000004</v>
+        <f t="shared" ref="G201:H201" si="41">(G$115*F201)/F$115</f>
+        <v>33688.744932134679</v>
       </c>
       <c r="H201" s="5">
-        <f t="shared" si="40"/>
-        <v>32500.000000000004</v>
+        <f t="shared" si="41"/>
+        <v>39751.34408602152</v>
       </c>
     </row>
     <row r="202" spans="2:9" ht="15.75" thickBot="1">
@@ -5543,24 +5560,24 @@
       </c>
       <c r="C202" s="57"/>
       <c r="D202" s="89">
-        <f t="shared" si="36"/>
-        <v>30000</v>
-      </c>
-      <c r="E202" s="35">
         <f t="shared" si="37"/>
         <v>30000</v>
       </c>
+      <c r="E202" s="35">
+        <f t="shared" si="38"/>
+        <v>30329.190904283445</v>
+      </c>
       <c r="F202" s="35">
-        <f t="shared" si="37"/>
-        <v>30000</v>
+        <f t="shared" si="38"/>
+        <v>30768.112109994712</v>
       </c>
       <c r="G202" s="35">
-        <f t="shared" ref="G202:H203" si="41">(G$115*F202)/F$115</f>
-        <v>30000</v>
+        <f t="shared" ref="G202:H203" si="42">(G$115*F202)/F$115</f>
+        <v>31097.303014278161</v>
       </c>
       <c r="H202" s="35">
-        <f t="shared" si="41"/>
-        <v>30000</v>
+        <f t="shared" si="42"/>
+        <v>36693.54838709678</v>
       </c>
     </row>
     <row r="203" spans="2:9" ht="15.75" thickBot="1">
@@ -5569,20 +5586,20 @@
         <v>176250</v>
       </c>
       <c r="E203" s="91">
-        <f t="shared" si="37"/>
-        <v>176250</v>
+        <f t="shared" si="38"/>
+        <v>178183.99656266527</v>
       </c>
       <c r="F203" s="91">
-        <f t="shared" si="37"/>
-        <v>176250</v>
+        <f t="shared" si="38"/>
+        <v>180762.65864621897</v>
       </c>
       <c r="G203" s="91">
-        <f t="shared" si="41"/>
-        <v>176250</v>
+        <f t="shared" si="42"/>
+        <v>182696.65520888424</v>
       </c>
       <c r="H203" s="92">
-        <f t="shared" si="41"/>
-        <v>176250</v>
+        <f t="shared" si="42"/>
+        <v>215574.59677419363</v>
       </c>
     </row>
     <row r="206" spans="2:9" ht="15.75" thickBot="1">
@@ -5615,20 +5632,20 @@
         <v>7830000</v>
       </c>
       <c r="E207" s="5">
-        <f t="shared" ref="E207:H207" si="42">E184*($I184+E198)*12</f>
-        <v>7830000</v>
+        <f t="shared" ref="E207:H207" si="43">E184*($I184+E198)*12</f>
+        <v>7839546.5362242199</v>
       </c>
       <c r="F207" s="5">
-        <f t="shared" si="42"/>
-        <v>7830000</v>
+        <f t="shared" si="43"/>
+        <v>7852275.2511898465</v>
       </c>
       <c r="G207" s="5">
-        <f t="shared" si="42"/>
-        <v>15660000</v>
+        <f t="shared" si="43"/>
+        <v>15723643.574828133</v>
       </c>
       <c r="H207" s="5">
-        <f t="shared" si="42"/>
-        <v>15660000</v>
+        <f t="shared" si="43"/>
+        <v>16048225.806451615</v>
       </c>
     </row>
     <row r="208" spans="2:9">
@@ -5637,24 +5654,24 @@
       </c>
       <c r="C208" s="32"/>
       <c r="D208" s="5">
-        <f t="shared" ref="D208:H211" si="43">D185*($I185+D199)*12</f>
+        <f t="shared" ref="D208:H211" si="44">D185*($I185+D199)*12</f>
         <v>9450000</v>
       </c>
       <c r="E208" s="5">
-        <f t="shared" si="43"/>
-        <v>9450000</v>
+        <f t="shared" si="44"/>
+        <v>9461521.6816499196</v>
       </c>
       <c r="F208" s="5">
-        <f t="shared" si="43"/>
-        <v>9450000</v>
+        <f t="shared" si="44"/>
+        <v>9476883.9238498155</v>
       </c>
       <c r="G208" s="5">
-        <f t="shared" si="43"/>
-        <v>18900000</v>
+        <f t="shared" si="44"/>
+        <v>18976811.21099947</v>
       </c>
       <c r="H208" s="5">
-        <f t="shared" si="43"/>
-        <v>18900000</v>
+        <f t="shared" si="44"/>
+        <v>19368548.387096774</v>
       </c>
     </row>
     <row r="209" spans="2:8">
@@ -5663,24 +5680,24 @@
       </c>
       <c r="C209" s="32"/>
       <c r="D209" s="5">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>7290000</v>
       </c>
       <c r="E209" s="5">
-        <f t="shared" si="43"/>
-        <v>7290000</v>
+        <f t="shared" si="44"/>
+        <v>7298888.1544156522</v>
       </c>
       <c r="F209" s="5">
-        <f t="shared" si="43"/>
-        <v>14580000</v>
+        <f t="shared" si="44"/>
+        <v>14621478.053939715</v>
       </c>
       <c r="G209" s="5">
-        <f t="shared" si="43"/>
-        <v>14580000</v>
+        <f t="shared" si="44"/>
+        <v>14639254.362771019</v>
       </c>
       <c r="H209" s="5">
-        <f t="shared" si="43"/>
-        <v>14580000</v>
+        <f t="shared" si="44"/>
+        <v>14941451.612903226</v>
       </c>
     </row>
     <row r="210" spans="2:8">
@@ -5689,24 +5706,24 @@
       </c>
       <c r="C210" s="32"/>
       <c r="D210" s="5">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>14040000</v>
       </c>
       <c r="E210" s="5">
-        <f t="shared" si="43"/>
-        <v>14040000</v>
+        <f t="shared" si="44"/>
+        <v>14057117.92702274</v>
       </c>
       <c r="F210" s="5">
-        <f t="shared" si="43"/>
-        <v>14040000</v>
+        <f t="shared" si="44"/>
+        <v>14079941.829719726</v>
       </c>
       <c r="G210" s="5">
-        <f t="shared" si="43"/>
-        <v>14040000</v>
+        <f t="shared" si="44"/>
+        <v>14097059.756742466</v>
       </c>
       <c r="H210" s="5">
-        <f t="shared" si="43"/>
-        <v>14040000</v>
+        <f t="shared" si="44"/>
+        <v>14388064.516129034</v>
       </c>
     </row>
     <row r="211" spans="2:8">
@@ -5715,24 +5732,24 @@
       </c>
       <c r="C211" s="32"/>
       <c r="D211" s="5">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>6480000</v>
       </c>
       <c r="E211" s="5">
-        <f t="shared" si="43"/>
-        <v>12960000</v>
+        <f t="shared" si="44"/>
+        <v>12975801.163405605</v>
       </c>
       <c r="F211" s="5">
-        <f t="shared" si="43"/>
-        <v>12960000</v>
+        <f t="shared" si="44"/>
+        <v>12996869.381279744</v>
       </c>
       <c r="G211" s="5">
-        <f t="shared" si="43"/>
-        <v>12960000</v>
+        <f t="shared" si="44"/>
+        <v>13012670.544685353</v>
       </c>
       <c r="H211" s="5">
-        <f t="shared" si="43"/>
-        <v>12960000</v>
+        <f t="shared" si="44"/>
+        <v>13281290.322580647</v>
       </c>
     </row>
     <row r="212" spans="2:8">
@@ -5741,23 +5758,23 @@
       </c>
       <c r="C212" s="32"/>
       <c r="D212" s="5">
-        <f t="shared" ref="D212:H213" si="44">D189*$I189*12</f>
+        <f t="shared" ref="D212:H213" si="45">D189*$I189*12</f>
         <v>13680000</v>
       </c>
       <c r="E212" s="5">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>13680000</v>
       </c>
       <c r="F212" s="5">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>13680000</v>
       </c>
       <c r="G212" s="5">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>13680000</v>
       </c>
       <c r="H212" s="5">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>13680000</v>
       </c>
     </row>
@@ -5767,23 +5784,23 @@
       </c>
       <c r="C213" s="32"/>
       <c r="D213" s="35">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>13200000</v>
       </c>
       <c r="E213" s="35">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>13200000</v>
       </c>
       <c r="F213" s="35">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>13200000</v>
       </c>
       <c r="G213" s="35">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>13200000</v>
       </c>
       <c r="H213" s="35">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>13200000</v>
       </c>
     </row>
@@ -5798,19 +5815,19 @@
       </c>
       <c r="E214" s="87">
         <f>SUM(E207:E213)</f>
-        <v>78450000</v>
+        <v>78512875.462718129</v>
       </c>
       <c r="F214" s="87">
-        <f t="shared" ref="F214:H214" si="45">SUM(F207:F213)</f>
-        <v>85740000</v>
+        <f t="shared" ref="F214:H214" si="46">SUM(F207:F213)</f>
+        <v>85907448.439978838</v>
       </c>
       <c r="G214" s="87">
-        <f t="shared" si="45"/>
-        <v>103020000</v>
+        <f t="shared" si="46"/>
+        <v>103329439.45002644</v>
       </c>
       <c r="H214" s="78">
-        <f t="shared" si="45"/>
-        <v>103020000</v>
+        <f t="shared" si="46"/>
+        <v>104907580.6451613</v>
       </c>
     </row>
   </sheetData>

</xml_diff>